<commit_message>
Data displayed in table format
</commit_message>
<xml_diff>
--- a/MajorProject.xlsx
+++ b/MajorProject.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKSHIT\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKSHIT\OneDrive\Desktop\CodeZone2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C4A3306-FF84-42F5-9A41-3EBBF264411C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287C510C-2B28-4A2A-8107-DA39A3EA049F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B628F232-8E39-4E35-B4F0-B9639D7FEB8D}"/>
   </bookViews>
@@ -56,9 +56,6 @@
     <t>Student C</t>
   </si>
   <si>
-    <t xml:space="preserve">SID D </t>
-  </si>
-  <si>
     <t>Student D</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>Dr. Manish</t>
+  </si>
+  <si>
+    <t>SID D</t>
   </si>
 </sst>
 </file>
@@ -453,7 +453,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,19 +491,19 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -514,34 +514,34 @@
         <v>18103001</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>18103011</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>18103021</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <v>18103031</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J2">
         <v>18103041</v>
       </c>
       <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
         <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -552,34 +552,34 @@
         <v>18103002</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3">
         <v>18103012</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3">
         <v>18103022</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>18103032</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3">
         <v>18103042</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -590,34 +590,34 @@
         <v>18103003</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>18103013</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4">
         <v>18103023</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4">
         <v>18103033</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4">
         <v>18103043</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -628,34 +628,34 @@
         <v>18103004</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>18103014</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5">
         <v>18103024</v>
       </c>
       <c r="G5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5">
         <v>18103034</v>
       </c>
       <c r="I5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5">
         <v>18103044</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -666,34 +666,34 @@
         <v>18103005</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6">
         <v>18103015</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6">
         <v>18103025</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6">
         <v>18103035</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J6">
         <v>18103045</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -704,34 +704,34 @@
         <v>18103006</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>18103016</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7">
         <v>18103026</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7">
         <v>18103036</v>
       </c>
       <c r="I7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J7">
         <v>18103046</v>
       </c>
       <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
         <v>16</v>
-      </c>
-      <c r="L7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -742,34 +742,34 @@
         <v>18103007</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8">
         <v>18103017</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>18103027</v>
       </c>
       <c r="G8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8">
         <v>18103037</v>
       </c>
       <c r="I8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J8">
         <v>18103047</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -780,34 +780,34 @@
         <v>18103008</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9">
         <v>18103018</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>18103028</v>
       </c>
       <c r="G9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H9">
         <v>18103038</v>
       </c>
       <c r="I9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9">
         <v>18103048</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -818,34 +818,34 @@
         <v>18103009</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10">
         <v>18103019</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>18103029</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10">
         <v>18103039</v>
       </c>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10">
         <v>18103049</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -856,34 +856,34 @@
         <v>18103010</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11">
         <v>18103020</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11">
         <v>18103030</v>
       </c>
       <c r="G11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H11">
         <v>18103040</v>
       </c>
       <c r="I11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J11">
         <v>18103050</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excell updated for testing purpose
</commit_message>
<xml_diff>
--- a/MajorProject.xlsx
+++ b/MajorProject.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKSHIT\OneDrive\Desktop\CodeZone2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287C510C-2B28-4A2A-8107-DA39A3EA049F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0DAD2E-3B9E-4A80-B677-8ADF1EE61099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B628F232-8E39-4E35-B4F0-B9639D7FEB8D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
   <si>
     <t>S.No.</t>
   </si>
@@ -83,22 +83,16 @@
     <t>E</t>
   </si>
   <si>
-    <t>Prof. Amandeep</t>
-  </si>
-  <si>
-    <t>Dr. Rupali Verma</t>
-  </si>
-  <si>
-    <t>Dr. Sachin Chaudhary</t>
-  </si>
-  <si>
-    <t>Prof. Rajesh Bhatia</t>
-  </si>
-  <si>
-    <t>Dr. Manish</t>
-  </si>
-  <si>
     <t>SID D</t>
+  </si>
+  <si>
+    <t>Akshit</t>
+  </si>
+  <si>
+    <t>Gagan</t>
+  </si>
+  <si>
+    <t>Shayan</t>
   </si>
 </sst>
 </file>
@@ -453,7 +447,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,7 +485,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -541,7 +535,7 @@
         <v>15</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -579,7 +573,7 @@
         <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -617,7 +611,7 @@
         <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -655,7 +649,7 @@
         <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -693,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -731,7 +725,7 @@
         <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -845,7 +839,7 @@
         <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -883,7 +877,7 @@
         <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Models/ save data updated
</commit_message>
<xml_diff>
--- a/MajorProject.xlsx
+++ b/MajorProject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKSHIT\OneDrive\Desktop\CodeZone2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gskhu\Downloads\CodeZone2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287C510C-2B28-4A2A-8107-DA39A3EA049F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6333D8CE-19F9-41FD-A4DE-BFCC118E069A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B628F232-8E39-4E35-B4F0-B9639D7FEB8D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{B628F232-8E39-4E35-B4F0-B9639D7FEB8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
   <si>
     <t>S.No.</t>
   </si>
@@ -83,22 +83,16 @@
     <t>E</t>
   </si>
   <si>
-    <t>Prof. Amandeep</t>
-  </si>
-  <si>
-    <t>Dr. Rupali Verma</t>
-  </si>
-  <si>
-    <t>Dr. Sachin Chaudhary</t>
-  </si>
-  <si>
-    <t>Prof. Rajesh Bhatia</t>
-  </si>
-  <si>
-    <t>Dr. Manish</t>
-  </si>
-  <si>
     <t>SID D</t>
+  </si>
+  <si>
+    <t>be18103032 Gaganpreet Singh Khurana</t>
+  </si>
+  <si>
+    <t>Akshit Garg</t>
+  </si>
+  <si>
+    <t>Shayan Yaseen</t>
   </si>
 </sst>
 </file>
@@ -453,7 +447,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,7 +485,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -541,7 +535,7 @@
         <v>15</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -579,7 +573,7 @@
         <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -617,7 +611,7 @@
         <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -655,7 +649,7 @@
         <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -693,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -731,7 +725,7 @@
         <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -769,7 +763,7 @@
         <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -807,7 +801,7 @@
         <v>15</v>
       </c>
       <c r="L9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -845,7 +839,7 @@
         <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -883,7 +877,7 @@
         <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Send mails working now
</commit_message>
<xml_diff>
--- a/MajorProject.xlsx
+++ b/MajorProject.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKSHIT\OneDrive\Desktop\CodeZone2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gskhu\Downloads\CodeZone2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE93D2EE-04CF-4D96-B6B9-B8E60E9D21E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650C46EA-12D5-4FCC-841E-8B0545FBD8E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B628F232-8E39-4E35-B4F0-B9639D7FEB8D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{B628F232-8E39-4E35-B4F0-B9639D7FEB8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="20">
   <si>
     <t>S.No.</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Shayan Yaseen</t>
+  </si>
+  <si>
+    <t>be18103032 Gaganpreet Singh Khurana</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,7 +535,7 @@
         <v>15</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -684,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -760,7 +763,7 @@
         <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -874,7 +877,7 @@
         <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>